<commit_message>
Added Plots for Kin + EMG
- Took all modified files from server
- Presentation 220623
</commit_message>
<xml_diff>
--- a/PRESENTATIONS/model_acc.xlsx
+++ b/PRESENTATIONS/model_acc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmartinez/Documents/GitHub/ObjectRecognition/PRESENTATIONS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327F52D-2806-BD47-A231-F242B94FE6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C261D-B9FA-4742-9B26-2A9A5BC5A73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47860" yWindow="-13300" windowWidth="19340" windowHeight="21100" activeTab="1" xr2:uid="{E5BF638B-22CC-7E4E-BC14-2958D53A395E}"/>
+    <workbookView xWindow="28800" yWindow="-880" windowWidth="38400" windowHeight="21100" firstSheet="1" activeTab="7" xr2:uid="{E5BF638B-22CC-7E4E-BC14-2958D53A395E}"/>
   </bookViews>
   <sheets>
     <sheet name="FitCECOC" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="SVM" sheetId="6" r:id="rId4"/>
     <sheet name="ANN" sheetId="7" r:id="rId5"/>
     <sheet name="All Syn" sheetId="8" r:id="rId6"/>
+    <sheet name="EMG" sheetId="9" r:id="rId7"/>
+    <sheet name="Kin + EMG" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
   <si>
     <t>MUGS</t>
   </si>
@@ -179,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,6 +203,9 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -519,7 +524,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="A5:H10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF08836C-2DA3-4247-BC60-003C6FD91B5B}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="H18:Q22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2078,7 +2083,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2127,18 +2132,36 @@
       <c r="B4" s="12">
         <v>43.85</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="C4" s="12">
+        <v>50.17</v>
+      </c>
+      <c r="D4" s="13">
+        <v>50.67</v>
+      </c>
+      <c r="E4" s="12">
+        <v>45.35</v>
+      </c>
+      <c r="F4" s="12">
+        <v>48.58</v>
+      </c>
+      <c r="G4" s="12">
+        <v>48.61</v>
+      </c>
+      <c r="H4" s="12">
+        <v>43.83</v>
+      </c>
+      <c r="I4" s="12">
+        <v>47.35</v>
+      </c>
+      <c r="J4" s="12">
+        <v>52.03</v>
+      </c>
+      <c r="K4" s="12">
+        <v>47.19</v>
+      </c>
       <c r="L4" s="6">
         <f>AVERAGE(B4:K4)</f>
-        <v>43.85</v>
+        <v>47.763000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2175,7 +2198,7 @@
       <c r="K5" s="12">
         <v>58.89</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="17">
         <f t="shared" ref="L5:L8" si="0">AVERAGE(B5:K5)</f>
         <v>59.134</v>
       </c>
@@ -2184,19 +2207,39 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="6" t="e">
+      <c r="B6" s="13">
+        <v>45.58</v>
+      </c>
+      <c r="C6" s="12">
+        <v>41.71</v>
+      </c>
+      <c r="D6" s="12">
+        <v>41.48</v>
+      </c>
+      <c r="E6" s="12">
+        <v>41.78</v>
+      </c>
+      <c r="F6" s="12">
+        <v>41.12</v>
+      </c>
+      <c r="G6" s="12">
+        <v>38.89</v>
+      </c>
+      <c r="H6" s="12">
+        <v>41.56</v>
+      </c>
+      <c r="I6" s="12">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="J6" s="12">
+        <v>39.06</v>
+      </c>
+      <c r="K6" s="12">
+        <v>43.46</v>
+      </c>
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>41.254999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2233,7 +2276,7 @@
       <c r="K7" s="12">
         <v>41.84</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="11">
         <f>AVERAGE(C7:K7)</f>
         <v>41.161111111111119</v>
       </c>
@@ -2280,44 +2323,745 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <f t="shared" ref="B9:J9" si="1">AVERAGE(B4:B8)</f>
-        <v>50.297499999999999</v>
+        <v>49.353999999999999</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="1"/>
-        <v>52.610000000000007</v>
-      </c>
-      <c r="D9" s="6">
-        <f t="shared" si="1"/>
-        <v>52.68</v>
+        <v>49.942</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>50.037999999999997</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>52.470000000000006</v>
+        <v>48.908000000000001</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="1"/>
-        <v>52.51</v>
+        <v>49.445999999999998</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="1"/>
-        <v>52.066666666666663</v>
+        <v>48.74</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>51.373333333333335</v>
+        <v>47.902000000000001</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="1"/>
-        <v>52.120000000000005</v>
+        <v>48.323999999999998</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="1"/>
-        <v>52.756666666666668</v>
+        <v>49.872</v>
       </c>
       <c r="K9" s="6">
         <f>AVERAGE(K4:K8)</f>
-        <v>51.82</v>
-      </c>
+        <v>49.221999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE8AE87-B9C1-5640-BA45-9A53882E85A2}">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>35.049999999999997</v>
+      </c>
+      <c r="C4" s="12">
+        <v>31.6</v>
+      </c>
+      <c r="D4" s="12">
+        <v>30.79</v>
+      </c>
+      <c r="E4" s="12">
+        <v>30.48</v>
+      </c>
+      <c r="F4" s="12">
+        <v>30.48</v>
+      </c>
+      <c r="G4" s="12">
+        <v>30.85</v>
+      </c>
+      <c r="H4" s="12">
+        <v>32.65</v>
+      </c>
+      <c r="I4" s="12">
+        <v>33.06</v>
+      </c>
+      <c r="J4" s="12">
+        <v>33.21</v>
+      </c>
+      <c r="K4" s="13">
+        <v>37.54</v>
+      </c>
+      <c r="L4" s="11">
+        <f>AVERAGE(B4:K4)</f>
+        <v>32.571000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>43.85</v>
+      </c>
+      <c r="C5" s="12">
+        <v>43.09</v>
+      </c>
+      <c r="D5" s="12">
+        <v>42.84</v>
+      </c>
+      <c r="E5" s="12">
+        <v>43.45</v>
+      </c>
+      <c r="F5" s="12">
+        <v>43.45</v>
+      </c>
+      <c r="G5" s="13">
+        <v>44.08</v>
+      </c>
+      <c r="H5" s="12">
+        <v>43.02</v>
+      </c>
+      <c r="I5" s="12">
+        <v>43.33</v>
+      </c>
+      <c r="J5" s="12">
+        <v>43.04</v>
+      </c>
+      <c r="K5" s="12">
+        <v>42.28</v>
+      </c>
+      <c r="L5" s="17">
+        <f t="shared" ref="L5:L8" si="0">AVERAGE(B5:K5)</f>
+        <v>43.242999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12">
+        <v>28.34</v>
+      </c>
+      <c r="C6" s="12">
+        <v>29.05</v>
+      </c>
+      <c r="D6" s="12">
+        <v>31.07</v>
+      </c>
+      <c r="E6" s="12">
+        <v>32.17</v>
+      </c>
+      <c r="F6" s="12">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="G6" s="12">
+        <v>37.64</v>
+      </c>
+      <c r="H6" s="12">
+        <v>30.52</v>
+      </c>
+      <c r="I6" s="12">
+        <v>38.24</v>
+      </c>
+      <c r="J6" s="12">
+        <v>38.78</v>
+      </c>
+      <c r="K6" s="13">
+        <v>39.82</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="0"/>
+        <v>34.292999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>28.98</v>
+      </c>
+      <c r="C7" s="12">
+        <v>29.71</v>
+      </c>
+      <c r="D7" s="12">
+        <v>31.07</v>
+      </c>
+      <c r="E7" s="12">
+        <v>32.17</v>
+      </c>
+      <c r="F7" s="12">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="G7" s="12">
+        <v>37.64</v>
+      </c>
+      <c r="H7" s="12">
+        <v>30.52</v>
+      </c>
+      <c r="I7" s="12">
+        <v>38.24</v>
+      </c>
+      <c r="J7" s="12">
+        <v>38.78</v>
+      </c>
+      <c r="K7" s="13">
+        <v>39.82</v>
+      </c>
+      <c r="L7" s="6">
+        <f>AVERAGE(C7:K7)</f>
+        <v>35.027777777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12">
+        <v>41.42</v>
+      </c>
+      <c r="C8" s="12">
+        <v>42.11</v>
+      </c>
+      <c r="D8" s="12">
+        <v>41.22</v>
+      </c>
+      <c r="E8" s="12">
+        <v>41.65</v>
+      </c>
+      <c r="F8" s="12">
+        <v>41.58</v>
+      </c>
+      <c r="G8" s="18">
+        <v>42.34</v>
+      </c>
+      <c r="H8" s="12">
+        <v>41.67</v>
+      </c>
+      <c r="I8" s="12">
+        <v>40.96</v>
+      </c>
+      <c r="J8" s="12">
+        <v>40.43</v>
+      </c>
+      <c r="K8" s="12">
+        <v>41.83</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="0"/>
+        <v>41.521000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <f t="shared" ref="B9:J9" si="1">AVERAGE(B4:B8)</f>
+        <v>35.527999999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>35.112000000000002</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>35.397999999999996</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="1"/>
+        <v>35.984000000000002</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="1"/>
+        <v>38.022000000000006</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>38.510000000000005</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="1"/>
+        <v>35.676000000000002</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>38.766000000000005</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>38.847999999999999</v>
+      </c>
+      <c r="K9" s="7">
+        <f>AVERAGE(K4:K8)</f>
+        <v>40.257999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="13"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+    </row>
+    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="13"/>
+    </row>
+    <row r="18" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+    </row>
+    <row r="20" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="F20" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFB6F69-9090-6A40-B729-AF591C4F55B4}">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:V19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13">
+        <v>47.67</v>
+      </c>
+      <c r="C4" s="12">
+        <v>47.02</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45.6</v>
+      </c>
+      <c r="E4" s="12">
+        <v>42.51</v>
+      </c>
+      <c r="F4" s="12">
+        <v>44.94</v>
+      </c>
+      <c r="G4" s="12">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="H4" s="12">
+        <v>45.15</v>
+      </c>
+      <c r="I4" s="12">
+        <v>46.26</v>
+      </c>
+      <c r="J4" s="12">
+        <v>43.39</v>
+      </c>
+      <c r="K4" s="12">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="L4" s="6">
+        <f>AVERAGE(B4:K4)</f>
+        <v>44.292999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>57</v>
+      </c>
+      <c r="C5" s="12">
+        <v>56.03</v>
+      </c>
+      <c r="D5" s="12">
+        <v>56.11</v>
+      </c>
+      <c r="E5" s="12">
+        <v>56.45</v>
+      </c>
+      <c r="F5" s="13">
+        <v>58.96</v>
+      </c>
+      <c r="G5" s="12">
+        <v>55.95</v>
+      </c>
+      <c r="H5" s="12">
+        <v>52.7</v>
+      </c>
+      <c r="I5" s="12">
+        <v>53.72</v>
+      </c>
+      <c r="J5" s="12">
+        <v>53.61</v>
+      </c>
+      <c r="K5" s="12">
+        <v>56.7</v>
+      </c>
+      <c r="L5" s="19">
+        <f t="shared" ref="L5:L8" si="0">AVERAGE(B5:K5)</f>
+        <v>55.722999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12">
+        <v>39.159999999999997</v>
+      </c>
+      <c r="C6" s="12">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="D6" s="12">
+        <v>39.29</v>
+      </c>
+      <c r="E6" s="12">
+        <v>42.48</v>
+      </c>
+      <c r="F6" s="13">
+        <v>43.33</v>
+      </c>
+      <c r="G6" s="12">
+        <v>37.85</v>
+      </c>
+      <c r="H6" s="12">
+        <v>40.159999999999997</v>
+      </c>
+      <c r="I6" s="12">
+        <v>36.130000000000003</v>
+      </c>
+      <c r="J6" s="12">
+        <v>32.54</v>
+      </c>
+      <c r="K6" s="12">
+        <v>41.61</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="0"/>
+        <v>39.332000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>38.840000000000003</v>
+      </c>
+      <c r="C7" s="12">
+        <v>41.35</v>
+      </c>
+      <c r="D7" s="12">
+        <v>41.72</v>
+      </c>
+      <c r="E7" s="13">
+        <v>42.73</v>
+      </c>
+      <c r="F7" s="12">
+        <v>41.85</v>
+      </c>
+      <c r="G7" s="12">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="H7" s="12">
+        <v>42.63</v>
+      </c>
+      <c r="I7" s="12">
+        <v>42.38</v>
+      </c>
+      <c r="J7" s="12">
+        <v>37.89</v>
+      </c>
+      <c r="K7" s="12">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="L7" s="11">
+        <f>AVERAGE(C7:K7)</f>
+        <v>41.025555555555549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12">
+        <v>51.34</v>
+      </c>
+      <c r="C8" s="12">
+        <v>51.16</v>
+      </c>
+      <c r="D8" s="12">
+        <v>39.22</v>
+      </c>
+      <c r="E8" s="12">
+        <v>48.07</v>
+      </c>
+      <c r="F8" s="12">
+        <v>50.62</v>
+      </c>
+      <c r="G8" s="12">
+        <v>50.45</v>
+      </c>
+      <c r="H8" s="13">
+        <v>53.06</v>
+      </c>
+      <c r="I8" s="12">
+        <v>49.71</v>
+      </c>
+      <c r="J8" s="12">
+        <v>51.32</v>
+      </c>
+      <c r="K8" s="12">
+        <v>46.18</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="0"/>
+        <v>49.113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <f t="shared" ref="B9:J9" si="1">AVERAGE(B4:B8)</f>
+        <v>46.802</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>47.266000000000005</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>44.387999999999998</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="1"/>
+        <v>46.447999999999993</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>47.940000000000005</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>44.841999999999999</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="1"/>
+        <v>46.739999999999995</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>45.64</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>43.75</v>
+      </c>
+      <c r="K9" s="6">
+        <f>AVERAGE(K4:K8)</f>
+        <v>44.720000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M15" s="13"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+    </row>
+    <row r="17" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+    </row>
+    <row r="18" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>